<commit_message>
more work on spreadsheets
</commit_message>
<xml_diff>
--- a/startup/doublewheel_template.xlsx
+++ b/startup/doublewheel_template.xlsx
@@ -909,9 +909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>516240</xdr:colOff>
+      <xdr:colOff>515880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -925,7 +925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2514600" cy="2738880"/>
+          <a:ext cx="2515680" cy="2738520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,9 +946,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>2033280</xdr:colOff>
+      <xdr:colOff>2032920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -957,8 +957,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3191400" y="6959880"/>
-          <a:ext cx="6642720" cy="2262960"/>
+          <a:off x="3192840" y="6959880"/>
+          <a:ext cx="6643440" cy="2262600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1092,7 +1092,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns Q,R,S; leave blank for no motion</a:t>
+            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1111,7 +1111,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Specify detector position in column T, blank means to </a:t>
+            <a:t>6. Specify detector position in column U, blank means to </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1167,7 +1167,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column AC</a:t>
+            <a:t>7. Do not add columns before column AD</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1207,14 +1207,14 @@
   <dimension ref="B1:AD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="L22" activeCellId="0" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -1229,9 +1229,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2450,9 +2450,9 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
tidy up double wheel template
</commit_message>
<xml_diff>
--- a/startup/doublewheel_template.xlsx
+++ b/startup/doublewheel_template.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -902,63 +902,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>515880</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>55440</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="6933960"/>
-          <a:ext cx="2515680" cy="2738520"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1166040</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2032920</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>327600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3192840" y="6959880"/>
-          <a:ext cx="6643440" cy="2262600"/>
+          <a:off x="3579120" y="8324640"/>
+          <a:ext cx="6643440" cy="2262240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1196,25 +1159,62 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676080</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1100520</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1291320" y="8316720"/>
+          <a:ext cx="1836720" cy="2449080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:AD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="L22" activeCellId="0" sqref="L22"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2353,83 +2353,79 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="18">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+  <dataValidations count="17">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:U9 T10:T30" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S30" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
       <formula1>10</formula1>
       <formula2>400</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R30" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
-      <formula1>-150</formula1>
-      <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6 U10:U30" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6" type="decimal">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:U72" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2440,7 +2436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2450,7 +2446,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -2515,7 +2511,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
more updates to double spreadsheet
</commit_message>
<xml_diff>
--- a/startup/doublewheel_template.xlsx
+++ b/startup/doublewheel_template.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
   <si>
     <t xml:space="preserve">Double wheel</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.5  0.5  0.5  0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inner</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -903,15 +906,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>297000</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:colOff>66600</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:colOff>96840</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -920,8 +923,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3579120" y="8324640"/>
-          <a:ext cx="6643440" cy="2262240"/>
+          <a:off x="3349440" y="10725120"/>
+          <a:ext cx="6643800" cy="2261880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,7 +1133,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column AD</a:t>
+            <a:t>7. Do not add columns before column AE</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1162,15 +1165,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>676440</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1100520</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1183,8 +1186,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1291320" y="8316720"/>
-          <a:ext cx="1836720" cy="2449080"/>
+          <a:off x="1292040" y="10772280"/>
+          <a:ext cx="1836360" cy="2448720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1204,17 +1207,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AD30"/>
+  <dimension ref="B1:AD54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q9" activeCellId="0" sqref="Q9"/>
+      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.01"/>
@@ -2337,6 +2340,798 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="59"/>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="50"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="54"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="55"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+      <c r="AA31" s="58"/>
+      <c r="AB31" s="59"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="50"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="53"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="54"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="55"/>
+      <c r="V32" s="56"/>
+      <c r="W32" s="57"/>
+      <c r="X32" s="57"/>
+      <c r="Y32" s="57"/>
+      <c r="Z32" s="57"/>
+      <c r="AA32" s="58"/>
+      <c r="AB32" s="59"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="47" t="n">
+        <v>3</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="54"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="55"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="57"/>
+      <c r="X33" s="57"/>
+      <c r="Y33" s="57"/>
+      <c r="Z33" s="57"/>
+      <c r="AA33" s="58"/>
+      <c r="AB33" s="59"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="28"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="54"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="55"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="57"/>
+      <c r="X34" s="57"/>
+      <c r="Y34" s="57"/>
+      <c r="Z34" s="57"/>
+      <c r="AA34" s="58"/>
+      <c r="AB34" s="59"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="28"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="54"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="54"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="56"/>
+      <c r="W35" s="57"/>
+      <c r="X35" s="57"/>
+      <c r="Y35" s="57"/>
+      <c r="Z35" s="57"/>
+      <c r="AA35" s="58"/>
+      <c r="AB35" s="59"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="28"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="54"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57"/>
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="58"/>
+      <c r="AB36" s="59"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="47" t="n">
+        <v>7</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="54"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="55"/>
+      <c r="V37" s="56"/>
+      <c r="W37" s="57"/>
+      <c r="X37" s="57"/>
+      <c r="Y37" s="57"/>
+      <c r="Z37" s="57"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="59"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="47" t="n">
+        <v>8</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="53"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="54"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="55"/>
+      <c r="V38" s="56"/>
+      <c r="W38" s="57"/>
+      <c r="X38" s="57"/>
+      <c r="Y38" s="57"/>
+      <c r="Z38" s="57"/>
+      <c r="AA38" s="58"/>
+      <c r="AB38" s="59"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="47" t="n">
+        <v>9</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="54"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="55"/>
+      <c r="V39" s="56"/>
+      <c r="W39" s="57"/>
+      <c r="X39" s="57"/>
+      <c r="Y39" s="57"/>
+      <c r="Z39" s="57"/>
+      <c r="AA39" s="58"/>
+      <c r="AB39" s="59"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="47" t="n">
+        <v>10</v>
+      </c>
+      <c r="C40" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="54"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="54"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="55"/>
+      <c r="V40" s="56"/>
+      <c r="W40" s="57"/>
+      <c r="X40" s="57"/>
+      <c r="Y40" s="57"/>
+      <c r="Z40" s="57"/>
+      <c r="AA40" s="58"/>
+      <c r="AB40" s="59"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="47" t="n">
+        <v>11</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="54"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="55"/>
+      <c r="V41" s="56"/>
+      <c r="W41" s="57"/>
+      <c r="X41" s="57"/>
+      <c r="Y41" s="57"/>
+      <c r="Z41" s="57"/>
+      <c r="AA41" s="58"/>
+      <c r="AB41" s="59"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="47" t="n">
+        <v>12</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="54"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="54"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="55"/>
+      <c r="V42" s="56"/>
+      <c r="W42" s="57"/>
+      <c r="X42" s="57"/>
+      <c r="Y42" s="57"/>
+      <c r="Z42" s="57"/>
+      <c r="AA42" s="58"/>
+      <c r="AB42" s="59"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="47" t="n">
+        <v>13</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="54"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="55"/>
+      <c r="V43" s="56"/>
+      <c r="W43" s="57"/>
+      <c r="X43" s="57"/>
+      <c r="Y43" s="57"/>
+      <c r="Z43" s="57"/>
+      <c r="AA43" s="58"/>
+      <c r="AB43" s="59"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="47" t="n">
+        <v>14</v>
+      </c>
+      <c r="C44" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="54"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="54"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="55"/>
+      <c r="V44" s="56"/>
+      <c r="W44" s="57"/>
+      <c r="X44" s="57"/>
+      <c r="Y44" s="57"/>
+      <c r="Z44" s="57"/>
+      <c r="AA44" s="58"/>
+      <c r="AB44" s="59"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="47" t="n">
+        <v>15</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="54"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="54"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="55"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="57"/>
+      <c r="X45" s="57"/>
+      <c r="Y45" s="57"/>
+      <c r="Z45" s="57"/>
+      <c r="AA45" s="58"/>
+      <c r="AB45" s="59"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="47" t="n">
+        <v>16</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="54"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="54"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="55"/>
+      <c r="V46" s="56"/>
+      <c r="W46" s="57"/>
+      <c r="X46" s="57"/>
+      <c r="Y46" s="57"/>
+      <c r="Z46" s="57"/>
+      <c r="AA46" s="58"/>
+      <c r="AB46" s="59"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="47" t="n">
+        <v>17</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="28"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="54"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="54"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="55"/>
+      <c r="V47" s="56"/>
+      <c r="W47" s="57"/>
+      <c r="X47" s="57"/>
+      <c r="Y47" s="57"/>
+      <c r="Z47" s="57"/>
+      <c r="AA47" s="58"/>
+      <c r="AB47" s="59"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="47" t="n">
+        <v>18</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="54"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="54"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="55"/>
+      <c r="V48" s="56"/>
+      <c r="W48" s="57"/>
+      <c r="X48" s="57"/>
+      <c r="Y48" s="57"/>
+      <c r="Z48" s="57"/>
+      <c r="AA48" s="58"/>
+      <c r="AB48" s="59"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="47" t="n">
+        <v>19</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="54"/>
+      <c r="O49" s="53"/>
+      <c r="P49" s="28"/>
+      <c r="Q49" s="54"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="55"/>
+      <c r="V49" s="56"/>
+      <c r="W49" s="57"/>
+      <c r="X49" s="57"/>
+      <c r="Y49" s="57"/>
+      <c r="Z49" s="57"/>
+      <c r="AA49" s="58"/>
+      <c r="AB49" s="59"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="C50" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="54"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="28"/>
+      <c r="Q50" s="54"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="55"/>
+      <c r="V50" s="56"/>
+      <c r="W50" s="57"/>
+      <c r="X50" s="57"/>
+      <c r="Y50" s="57"/>
+      <c r="Z50" s="57"/>
+      <c r="AA50" s="58"/>
+      <c r="AB50" s="59"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="47" t="n">
+        <v>21</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="53"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="54"/>
+      <c r="O51" s="53"/>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="54"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="55"/>
+      <c r="V51" s="56"/>
+      <c r="W51" s="57"/>
+      <c r="X51" s="57"/>
+      <c r="Y51" s="57"/>
+      <c r="Z51" s="57"/>
+      <c r="AA51" s="58"/>
+      <c r="AB51" s="59"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="47" t="n">
+        <v>22</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="47"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="54"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="28"/>
+      <c r="Q52" s="54"/>
+      <c r="T52" s="9"/>
+      <c r="U52" s="55"/>
+      <c r="V52" s="56"/>
+      <c r="W52" s="57"/>
+      <c r="X52" s="57"/>
+      <c r="Y52" s="57"/>
+      <c r="Z52" s="57"/>
+      <c r="AA52" s="58"/>
+      <c r="AB52" s="59"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="47" t="n">
+        <v>23</v>
+      </c>
+      <c r="C53" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="51"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="54"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="54"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="55"/>
+      <c r="V53" s="56"/>
+      <c r="W53" s="57"/>
+      <c r="X53" s="57"/>
+      <c r="Y53" s="57"/>
+      <c r="Z53" s="57"/>
+      <c r="AA53" s="58"/>
+      <c r="AB53" s="59"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="47" t="n">
+        <v>24</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="54"/>
+      <c r="O54" s="53"/>
+      <c r="P54" s="28"/>
+      <c r="Q54" s="54"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="55"/>
+      <c r="V54" s="56"/>
+      <c r="W54" s="57"/>
+      <c r="X54" s="57"/>
+      <c r="Y54" s="57"/>
+      <c r="Z54" s="57"/>
+      <c r="AA54" s="58"/>
+      <c r="AB54" s="59"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="B1:D1"/>
@@ -2354,27 +3149,27 @@
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA54" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J54" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K54" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F54" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B54" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 D6:D54" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2394,7 +3189,7 @@
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H54" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2406,7 +3201,7 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I54" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2414,7 +3209,7 @@
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C54" type="list">
       <formula1>"Outer,Inner,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2446,7 +3241,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -2454,10 +3249,10 @@
   <sheetData>
     <row r="1" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +3268,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,7 +3276,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2489,7 +3284,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,7 +3292,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +3300,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>